<commit_message>
C02_Mercedes class'inda calismalar yapildi.
</commit_message>
<xml_diff>
--- a/src/test/java/resources/ulkeler.xlsx
+++ b/src/test/java/resources/ulkeler.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9DA0FD-1E54-457F-AF3B-C5FD0A0ECFD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593DA80F-72F0-4005-88D1-07FB909608FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-105" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="764" uniqueCount="573">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="574">
   <si>
     <t>Ülke (İngilizce)</t>
   </si>
@@ -1741,12 +1741,16 @@
   </si>
   <si>
     <t>Zimbabve</t>
+  </si>
+  <si>
+    <t>Nufus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2167,15 +2171,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D191"/>
+  <dimension ref="A1:E191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="25.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="4" customWidth="true" width="25.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2191,6 +2195,9 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s" s="0">
+        <v>573</v>
+      </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -2205,6 +2212,9 @@
       <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="E2" t="n" s="0">
+        <v>1500000.0</v>
+      </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
@@ -2317,6 +2327,9 @@
       <c r="D10" s="8" t="s">
         <v>30</v>
       </c>
+      <c r="E10" t="n" s="0">
+        <v>250000.0</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
@@ -2386,6 +2399,9 @@
       </c>
       <c r="D15" s="7" t="s">
         <v>49</v>
+      </c>
+      <c r="E15" t="n" s="0">
+        <v>54000.0</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>